<commit_message>
welcome to the new age
</commit_message>
<xml_diff>
--- a/backend/uploads/tables/form1.xlsx
+++ b/backend/uploads/tables/form1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\А078\Desktop\Web\nosql2h24-yandex\backend\uploads\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\А078\Desktop\123\nosql2h24-yandex\backend\uploads\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C03C42-8078-478B-89E3-7A7F247B7511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA11617-420C-4E8F-A617-A1703895C195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6030" yWindow="1575" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6060" yWindow="1620" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>ID</t>
   </si>
@@ -56,13 +56,46 @@
   </si>
   <si>
     <t>Это кошка?</t>
+  </si>
+  <si>
+    <t>2024-12-01 10:23:25</t>
+  </si>
+  <si>
+    <t>2024-12-01 10:23:29</t>
+  </si>
+  <si>
+    <t>2024-12-10 15:00:00</t>
+  </si>
+  <si>
+    <t>2024-12-10 15:00:01</t>
+  </si>
+  <si>
+    <t>2024-12-15 23:02:02</t>
+  </si>
+  <si>
+    <t>2024-12-15 23:02:03</t>
+  </si>
+  <si>
+    <t>1898367659</t>
+  </si>
+  <si>
+    <t>1898367632</t>
+  </si>
+  <si>
+    <t>1898367594</t>
+  </si>
+  <si>
+    <t>1898367660</t>
+  </si>
+  <si>
+    <t>1898367665</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,6 +106,11 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,9 +133,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -327,71 +367,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>

</xml_diff>